<commit_message>
test buildings in scene
</commit_message>
<xml_diff>
--- a/static/Needs Table.xlsx
+++ b/static/Needs Table.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="12105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="12105" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Needs" sheetId="1" r:id="rId1"/>
     <sheet name="Interactions" sheetId="2" r:id="rId2"/>
+    <sheet name="Buildings" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -449,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -511,4 +512,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>